<commit_message>
Added more old transcripts
</commit_message>
<xml_diff>
--- a/sources/oyez/cases/conlaw.xlsx
+++ b/sources/oyez/cases/conlaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/Sites/loners/lonedissent/sources/oyez/cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F64A426-73EE-AC4D-A600-51417612BAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB121286-4539-0141-975B-69A0D2B72BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="840" windowWidth="26360" windowHeight="17440" xr2:uid="{D03C7472-E9A2-7344-8FBB-D623DD0FEEEE}"/>
+    <workbookView xWindow="5660" yWindow="2320" windowWidth="26360" windowHeight="17440" xr2:uid="{D03C7472-E9A2-7344-8FBB-D623DD0FEEEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6655" uniqueCount="3446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6656" uniqueCount="3446">
   <si>
     <t>Title</t>
   </si>
@@ -10799,8 +10799,8 @@
   <dimension ref="A1:AG952"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A940" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F952" sqref="F952"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20195,6 +20195,9 @@
       <c r="B99" s="2">
         <v>11</v>
       </c>
+      <c r="C99" s="2" t="s">
+        <v>1266</v>
+      </c>
       <c r="D99" s="3" t="s">
         <v>506</v>
       </c>

</xml_diff>